<commit_message>
UP to date gemaakt
</commit_message>
<xml_diff>
--- a/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
+++ b/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 47" sheetId="1" r:id="rId1"/>
     <sheet name="week 48" sheetId="2" r:id="rId2"/>
     <sheet name="week 50" sheetId="5" r:id="rId3"/>
     <sheet name="week 2" sheetId="6" r:id="rId4"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId5"/>
+    <sheet name="week 4" sheetId="7" r:id="rId5"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Logboek</t>
   </si>
@@ -143,6 +144,9 @@
   </si>
   <si>
     <t>Activatie van de mail aan het regelen en mailtje zelf gemaakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bijgewerkt naar leraars project </t>
   </si>
 </sst>
 </file>
@@ -1633,7 +1637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1990,6 +1994,322 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="3"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41669</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="9">
+        <f>D7-C7</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9">
+        <f t="shared" ref="G9:G18" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="9">
+        <f t="shared" ref="G20:G25" si="1">D20-C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9">
+        <f>SUM(G7:G22)</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>

</xml_diff>

<commit_message>
bezig met upload_form met thumbnail
</commit_message>
<xml_diff>
--- a/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
+++ b/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 47" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,15 @@
     <sheet name="week 50" sheetId="5" r:id="rId3"/>
     <sheet name="week 2" sheetId="6" r:id="rId4"/>
     <sheet name="week 4" sheetId="7" r:id="rId5"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId6"/>
+    <sheet name="week 7" sheetId="9" r:id="rId6"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
   <si>
     <t>Logboek</t>
   </si>
@@ -165,6 +166,9 @@
   </si>
   <si>
     <t>Bezig met comentaar in LoginClass.php</t>
+  </si>
+  <si>
+    <t>bezig in upload_form</t>
   </si>
 </sst>
 </file>
@@ -174,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,23 +570,23 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="2" max="2" width="9.625" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="2"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.75" customWidth="1"/>
-    <col min="7" max="7" width="8.875" style="2"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -590,7 +594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -598,7 +602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -606,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -630,7 +634,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="28.5">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -655,7 +659,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="28.5">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -676,7 +680,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9"/>
@@ -691,7 +695,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9"/>
@@ -706,7 +710,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="9"/>
@@ -721,7 +725,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9"/>
@@ -735,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9"/>
@@ -749,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8">
@@ -761,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8">
@@ -773,14 +777,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8">
@@ -792,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -804,14 +808,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -824,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -836,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -849,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -859,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -869,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -879,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
@@ -905,15 +909,15 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="3"/>
-    <col min="6" max="6" width="37.75" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="3"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -932,7 +936,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -943,7 +947,7 @@
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -954,12 +958,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -983,7 +987,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1008,7 +1012,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="28.5">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -1029,7 +1033,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="42.75">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9">
@@ -1050,7 +1054,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9"/>
@@ -1060,7 +1064,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1085,7 +1089,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9">
@@ -1105,7 +1109,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9">
@@ -1125,7 +1129,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9">
         <v>0.47222222222222227</v>
       </c>
@@ -1143,7 +1147,7 @@
         <v>2.7777777777777735E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="42.75">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="9">
         <v>0.5</v>
       </c>
@@ -1161,14 +1165,14 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8">
@@ -1180,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -1192,14 +1196,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1212,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -1224,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -1237,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1247,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -1257,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1267,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -1291,15 +1295,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="37.75" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1311,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1318,7 +1322,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1329,7 +1333,7 @@
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1340,12 +1344,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1369,7 +1373,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1394,7 +1398,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9"/>
@@ -1404,7 +1408,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1429,7 +1433,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="28.5">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9">
@@ -1450,7 +1454,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="9">
@@ -1471,7 +1475,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="28.5">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9">
@@ -1491,7 +1495,7 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9"/>
@@ -1505,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8">
@@ -1517,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8">
@@ -1529,14 +1533,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8">
@@ -1548,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8">
@@ -1560,14 +1564,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1580,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8">
@@ -1592,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -1605,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1615,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -1625,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1635,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -1659,15 +1663,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="37.75" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1675,7 +1679,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1686,7 +1690,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1697,7 +1701,7 @@
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1708,12 +1712,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1737,7 +1741,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1766,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="28.5">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -1780,7 +1784,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="28.5">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
       <c r="C9" s="9">
@@ -1801,7 +1805,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9"/>
@@ -1814,7 +1818,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="42.75">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1839,7 +1843,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9">
@@ -1859,7 +1863,7 @@
         <v>1.7361111111111049E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.5">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9">
@@ -1879,7 +1883,7 @@
         <v>1200.0625</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8"/>
@@ -1889,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -1899,14 +1903,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -1916,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
@@ -1926,14 +1930,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1944,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -1954,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -1965,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1975,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -1985,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1995,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -2015,19 +2019,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="37.75" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2035,7 +2039,7 @@
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2050,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2057,7 +2061,7 @@
       <c r="D3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2068,12 +2072,12 @@
       <c r="D4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2101,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2122,7 +2126,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9">
@@ -2143,7 +2147,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
       <c r="C9" s="9"/>
@@ -2156,7 +2160,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2185,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="9">
@@ -2202,7 +2206,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="9">
@@ -2222,7 +2226,7 @@
         <v>2.0833333333333315E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="9">
@@ -2242,7 +2246,7 @@
         <v>2.0833333333333315E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9">
         <v>0.45833333333333331</v>
       </c>
@@ -2260,7 +2264,7 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -2270,14 +2274,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -2287,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
@@ -2297,14 +2301,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2315,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -2325,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
@@ -2336,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -2346,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -2356,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -2366,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -2384,25 +2388,358 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41681</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="9">
+        <f>D7-C7</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9">
+        <f>D8-C8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9">
+        <f t="shared" ref="G9:G18" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8">
+        <v>6</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8">
+        <v>7</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="9">
+        <f t="shared" ref="G20:G25" si="1">D20-C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9">
+        <f>SUM(G7:G22)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2412,7 +2749,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2422,7 +2759,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2432,7 +2769,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -2440,7 +2777,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>47</v>
       </c>
@@ -2449,13 +2786,13 @@
         <v>6.5972222222222265E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>48</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Mogelijk gemaakt om bestanden weg te laten schijven
</commit_message>
<xml_diff>
--- a/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
+++ b/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="52">
   <si>
     <t>Logboek</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>thumbnail bezig</t>
+  </si>
+  <si>
+    <t>Dinsdag</t>
+  </si>
+  <si>
+    <t>Mogelijk gemaakt om bestanden weg te laten schijven</t>
+  </si>
+  <si>
+    <t>Jquery gedownload</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,7 +2486,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5">
         <v>41681</v>
@@ -2521,33 +2530,49 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="12"/>
+      <c r="C9" s="9">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="G9" s="9">
         <f t="shared" ref="G9:G18" si="0">D9-C9</f>
-        <v>0</v>
+        <v>5.2083333333333315E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="5">
+        <v>41683</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E10" s="8">
-        <v>3</v>
-      </c>
-      <c r="F10" s="12"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G10" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -2556,9 +2581,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="8">
-        <v>4</v>
-      </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="12"/>
       <c r="G11" s="9">
         <f t="shared" si="0"/>
@@ -2571,9 +2594,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="8">
-        <v>5</v>
-      </c>
+      <c r="E12" s="8"/>
       <c r="F12" s="12"/>
       <c r="G12" s="9">
         <f t="shared" si="0"/>
@@ -2585,9 +2606,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="8">
-        <v>6</v>
-      </c>
+      <c r="E13" s="8"/>
       <c r="F13" s="12"/>
       <c r="G13" s="9">
         <f t="shared" si="0"/>
@@ -2597,9 +2616,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="8">
-        <v>7</v>
-      </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="12"/>
       <c r="G14" s="9">
         <f t="shared" si="0"/>
@@ -2720,7 +2737,7 @@
       </c>
       <c r="G26" s="9">
         <f>SUM(G7:G22)</f>
-        <v>7.2916666666666685E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bezig met bekijk pagina fotos
</commit_message>
<xml_diff>
--- a/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
+++ b/Logboek en ProjectOpdracht/logboekFotosjaak.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="10710" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 47" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="week 2" sheetId="6" r:id="rId4"/>
     <sheet name="week 4" sheetId="7" r:id="rId5"/>
     <sheet name="week 7" sheetId="9" r:id="rId6"/>
-    <sheet name="Totaal" sheetId="3" r:id="rId7"/>
+    <sheet name="week 10" sheetId="10" r:id="rId7"/>
+    <sheet name="Totaal" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="53">
   <si>
     <t>Logboek</t>
   </si>
@@ -181,6 +182,9 @@
   </si>
   <si>
     <t>Jquery gedownload</t>
+  </si>
+  <si>
+    <t>bezig met fout eruit te halen</t>
   </si>
 </sst>
 </file>
@@ -2402,7 +2406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2746,6 +2750,331 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41732</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="9">
+        <f>D7-C7</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9">
+        <f>D8-C8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9">
+        <f t="shared" ref="G9:G18" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="9">
+        <f t="shared" ref="G20:G25" si="1">D20-C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9">
+        <f>SUM(G7:G22)</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>

</xml_diff>